<commit_message>
updated coding sheet to start
</commit_message>
<xml_diff>
--- a/Article Coding/Count - Logistic Article Coding Sheet.xlsx
+++ b/Article Coding/Count - Logistic Article Coding Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin King\Documents\GitHub\glm_int\Key Manuscripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\GitHub\glm_main\Article Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DB2CC3-2361-4D19-8C70-66830645B42D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EA407A13-3DB7-41DE-997D-A76C5544891C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{04AE24AD-208A-4845-90BB-1147D10A6039}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{04AE24AD-208A-4845-90BB-1147D10A6039}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Result #</t>
   </si>
   <si>
-    <t>Relevant Analysis (Y/N)</t>
-  </si>
-  <si>
-    <t>Outcome Type</t>
-  </si>
-  <si>
     <t>Interpret conditional effects</t>
   </si>
   <si>
@@ -48,12 +42,6 @@
     <t>Multinomial logistic regression</t>
   </si>
   <si>
-    <t>Report Transformed OR/RR</t>
-  </si>
-  <si>
-    <t>Coefficient Figure</t>
-  </si>
-  <si>
     <t>Pois</t>
   </si>
   <si>
@@ -121,6 +109,36 @@
   </si>
   <si>
     <t>Zero-Inflated Negative Binomial</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Coefficient figure</t>
+  </si>
+  <si>
+    <t>Report transformed OR/RR</t>
+  </si>
+  <si>
+    <t>Outcome type</t>
+  </si>
+  <si>
+    <t>Relevant analysis (Y/N)</t>
+  </si>
+  <si>
+    <t>Examined distributions</t>
+  </si>
+  <si>
+    <t>Reported effect in terms of count or probability</t>
+  </si>
+  <si>
+    <t>Discussed centering</t>
+  </si>
+  <si>
+    <t>Justification for Y transformation</t>
+  </si>
+  <si>
+    <t>Total sample size (n)</t>
   </si>
 </sst>
 </file>
@@ -172,7 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -180,7 +198,13 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -497,452 +521,471 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C4D847-FF09-4AF9-ACBE-A05749726084}">
-  <dimension ref="A2:K58"/>
+  <dimension ref="A2:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G58"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="15.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="42.5546875" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <f>COUNTIF(C4:C60,"Y")</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="e">
+        <f>COUNTIF(E4:E58,"Yes")/COUNTIF($C4:$C58,"Y")</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F2" s="5" t="e">
+        <f>ROUND(COUNTIF(F4:F58,"Yes")/COUNTIF($C4:$C58,"Y")*100,2)&amp;"% / " &amp; ROUND(COUNTIF(F4:F58,"Yes (Int)")/COUNTIF($C4:$C58,"Y")*100,2)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G2" s="4" t="e">
+        <f>COUNTIF(G4:G58,"Yes")/COUNTIF($C4:$C58,"Y")</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="3" t="e">
+        <f>COUNTIF(D:D,P3)/COUNTIF($C4:$C58,"Y")</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3" t="e">
+        <f t="shared" ref="O4:O11" si="0">COUNTIF(D:D,P4)/COUNTIF($C5:$C59,"Y")</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="O5" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="O6" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="O7" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="O8" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="O9" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="O10" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="O11" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
-        <f>COUNTIF(B4:B60,"Y")</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="e">
-        <f>COUNTIF(D4:D58,"Yes")/COUNTIF($B4:$B58,"Y")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E2" s="4" t="e">
-        <f>ROUND(COUNTIF(E4:E58,"Yes")/COUNTIF($B4:$B58,"Y")*100,2)&amp;"% / " &amp; ROUND(COUNTIF(E4:E58,"Yes (Int)")/COUNTIF($B4:$B58,"Y")*100,2)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F2" s="3" t="e">
-        <f>COUNTIF(F4:F58,"Yes")/COUNTIF($B4:$B58,"Y")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="P17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="P18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="P19" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="3" t="e">
-        <f>COUNTIF(C:C,J3)/COUNTIF($B4:$B58,"Y")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3" t="e">
-        <f t="shared" ref="I4:I11" si="0">COUNTIF(C:C,J4)/COUNTIF($B5:$B59,"Y")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="I5" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="I6" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="I7" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" t="s">
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>17</v>
       </c>
-      <c r="K7" t="s">
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="I8" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" t="s">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27">
         <v>24</v>
       </c>
-      <c r="K8" t="s">
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="I9" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" t="s">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29">
         <v>26</v>
       </c>
-      <c r="K9" t="s">
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="I10" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" t="s">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31">
         <v>28</v>
       </c>
-      <c r="K10" t="s">
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="I11" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33">
         <v>30</v>
       </c>
-      <c r="K11" t="s">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="J17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="J18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="J19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58">
         <v>55</v>
       </c>
     </row>

</xml_diff>